<commit_message>
Modulo de pago de orden
</commit_message>
<xml_diff>
--- a/backend/database/seeders/Catalogos/RolMenu.xlsx
+++ b/backend/database/seeders/Catalogos/RolMenu.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\hotel_restuarante\backend\database\seeders\Catalogos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\restaurante-hotel\backend\database\seeders\Catalogos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="82">
   <si>
     <t>#</t>
   </si>
@@ -267,13 +267,16 @@
   </si>
   <si>
     <t>payment</t>
+  </si>
+  <si>
+    <t>Administrar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,6 +293,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <u/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
@@ -315,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -331,6 +340,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -613,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -781,10 +793,10 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="C9" t="s">
         <v>23</v>
@@ -793,7 +805,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>15</v>
@@ -801,19 +813,19 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>81</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>50</v>
+      <c r="E10" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>15</v>
@@ -821,19 +833,19 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>81</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>15</v>
@@ -841,19 +853,19 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>81</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>15</v>
@@ -861,19 +873,19 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>81</v>
       </c>
       <c r="D13" s="4">
         <v>1</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>15</v>
@@ -881,19 +893,19 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>81</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>15</v>
@@ -901,10 +913,10 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
         <v>23</v>
@@ -913,7 +925,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>15</v>
@@ -921,10 +933,10 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
         <v>23</v>
@@ -933,44 +945,44 @@
         <v>1</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F16" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>0</v>
+        <v>35</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
       </c>
       <c r="D17" s="4">
         <v>1</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" t="s">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>15</v>
@@ -978,10 +990,10 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
         <v>39</v>
@@ -990,7 +1002,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>15</v>
@@ -998,10 +1010,10 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
         <v>39</v>
@@ -1010,7 +1022,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>15</v>
@@ -1018,10 +1030,10 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C21" t="s">
         <v>39</v>
@@ -1030,7 +1042,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>15</v>
@@ -1038,10 +1050,10 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="C22" t="s">
         <v>39</v>
@@ -1050,7 +1062,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>15</v>
@@ -1058,19 +1070,19 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B23" t="s">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="D23" s="4">
         <v>1</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>15</v>
@@ -1078,10 +1090,10 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B24" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C24" t="s">
         <v>62</v>
@@ -1090,7 +1102,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>15</v>
@@ -1098,10 +1110,10 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C25" t="s">
         <v>62</v>
@@ -1110,7 +1122,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>15</v>
@@ -1118,10 +1130,10 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
         <v>62</v>
@@ -1130,7 +1142,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>15</v>
@@ -1138,10 +1150,10 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C27" t="s">
         <v>62</v>
@@ -1150,7 +1162,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>15</v>
@@ -1158,10 +1170,10 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C28" t="s">
         <v>62</v>
@@ -1169,10 +1181,30 @@
       <c r="D28" s="4">
         <v>1</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="4">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
         <v>75</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Empleados, Clientes y Proveedores funcionando.
</commit_message>
<xml_diff>
--- a/backend/database/seeders/Catalogos/RolMenu.xlsx
+++ b/backend/database/seeders/Catalogos/RolMenu.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\restaurante-hotel\backend\database\seeders\Catalogos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\hotel_restuarante\backend\database\seeders\Catalogos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="108">
   <si>
     <t>#</t>
   </si>
@@ -276,6 +276,78 @@
   </si>
   <si>
     <t>inventario</t>
+  </si>
+  <si>
+    <t>Caja Chica</t>
+  </si>
+  <si>
+    <t>Clientes</t>
+  </si>
+  <si>
+    <t>clientes</t>
+  </si>
+  <si>
+    <t>account_box</t>
+  </si>
+  <si>
+    <t>people_alt</t>
+  </si>
+  <si>
+    <t>Proveedores</t>
+  </si>
+  <si>
+    <t>proveedores</t>
+  </si>
+  <si>
+    <t>lock_open</t>
+  </si>
+  <si>
+    <t>Bitácora</t>
+  </si>
+  <si>
+    <t>bitacora</t>
+  </si>
+  <si>
+    <t>bug_report</t>
+  </si>
+  <si>
+    <t>table_chart</t>
+  </si>
+  <si>
+    <t>reportes</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>dashboard_hotel</t>
+  </si>
+  <si>
+    <t>dashboard</t>
+  </si>
+  <si>
+    <t>Empleados</t>
+  </si>
+  <si>
+    <t>empleados</t>
+  </si>
+  <si>
+    <t>badge</t>
+  </si>
+  <si>
+    <t>Apertura de caja</t>
+  </si>
+  <si>
+    <t>apertura_caja_hotel</t>
+  </si>
+  <si>
+    <t>caja_chica_hotel</t>
+  </si>
+  <si>
+    <t>Cierre de caja</t>
+  </si>
+  <si>
+    <t>cierre_caja_hotel</t>
   </si>
 </sst>
 </file>
@@ -622,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -663,35 +735,38 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" ht="21">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>101</v>
       </c>
       <c r="D2" s="4">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>102</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>16</v>
+      <c r="E3" t="s">
+        <v>20</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>15</v>
@@ -699,19 +774,16 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>85</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
-        <v>16</v>
+      <c r="E4" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>15</v>
@@ -719,16 +791,16 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
       </c>
-      <c r="E5" t="s">
-        <v>9</v>
+      <c r="E5" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>15</v>
@@ -736,7 +808,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
@@ -744,8 +816,8 @@
       <c r="D6" s="4">
         <v>1</v>
       </c>
-      <c r="E6" t="s">
-        <v>1</v>
+      <c r="E6" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>15</v>
@@ -753,19 +825,19 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D7" s="4">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>15</v>
@@ -773,16 +845,16 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D8" s="4">
         <v>1</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>48</v>
+      <c r="E8" t="s">
+        <v>9</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>15</v>
@@ -790,18 +862,15 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>76</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
       </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
       <c r="D9" s="4">
         <v>1</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" t="s">
         <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -810,19 +879,19 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>76</v>
+        <v>8</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>77</v>
+      <c r="E10" t="s">
+        <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>15</v>
@@ -830,19 +899,16 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>15</v>
@@ -850,19 +916,19 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>23</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>77</v>
+        <v>1</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>15</v>
@@ -870,10 +936,10 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
         <v>76</v>
@@ -890,10 +956,10 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
         <v>76</v>
@@ -910,19 +976,19 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="D15" s="4">
         <v>1</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>15</v>
@@ -930,19 +996,19 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="D16" s="4">
         <v>1</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>15</v>
@@ -950,19 +1016,19 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="D17" s="4">
         <v>1</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>15</v>
@@ -970,10 +1036,10 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
         <v>23</v>
@@ -982,124 +1048,124 @@
         <v>1</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="4" t="s">
-        <v>79</v>
+      <c r="A19" t="s">
+        <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="D19" s="4">
         <v>1</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="F19" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="4" t="s">
-        <v>82</v>
+      <c r="A20" t="s">
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>83</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="B21" t="s">
         <v>0</v>
       </c>
+      <c r="C21" t="s">
+        <v>23</v>
+      </c>
       <c r="D21" s="4">
         <v>1</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" t="s">
-        <v>40</v>
+      <c r="A22" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="D22" s="4">
         <v>1</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F22" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" t="s">
-        <v>42</v>
+      <c r="A23" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="D23" s="4">
         <v>1</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" t="s">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="D24" s="4">
         <v>1</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>15</v>
@@ -1107,10 +1173,10 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>97</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>98</v>
       </c>
       <c r="C25" t="s">
         <v>39</v>
@@ -1119,7 +1185,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>15</v>
@@ -1127,10 +1193,10 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s">
         <v>39</v>
@@ -1139,7 +1205,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>15</v>
@@ -1147,19 +1213,19 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="C27" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="D27" s="4">
         <v>1</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>15</v>
@@ -1167,19 +1233,19 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="C28" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="D28" s="4">
         <v>1</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>15</v>
@@ -1187,19 +1253,19 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="C29" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="D29" s="4">
         <v>1</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>15</v>
@@ -1207,19 +1273,19 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B30" t="s">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="C30" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="D30" s="4">
         <v>1</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>15</v>
@@ -1227,10 +1293,10 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B31" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="C31" t="s">
         <v>57</v>
@@ -1239,7 +1305,7 @@
         <v>1</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>15</v>
@@ -1247,10 +1313,10 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B32" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C32" t="s">
         <v>57</v>
@@ -1258,10 +1324,187 @@
       <c r="D32" s="4">
         <v>1</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" t="s">
+        <v>57</v>
+      </c>
+      <c r="D33" s="4">
+        <v>1</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" s="4">
+        <v>1</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="4">
+        <v>1</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" t="s">
+        <v>57</v>
+      </c>
+      <c r="D36" s="4">
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
         <v>70</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="F36" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="4">
+        <v>1</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>103</v>
+      </c>
+      <c r="B38" t="s">
+        <v>104</v>
+      </c>
+      <c r="C38" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" s="4">
+        <v>0</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>106</v>
+      </c>
+      <c r="B39" t="s">
+        <v>107</v>
+      </c>
+      <c r="C39" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39" s="4">
+        <v>0</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" s="4">
+        <v>1</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>92</v>
+      </c>
+      <c r="B41" t="s">
+        <v>93</v>
+      </c>
+      <c r="D41" s="4">
+        <v>1</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Creacion modulo de caja
</commit_message>
<xml_diff>
--- a/backend/database/seeders/Catalogos/RolMenu.xlsx
+++ b/backend/database/seeders/Catalogos/RolMenu.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="113">
   <si>
     <t>#</t>
   </si>
@@ -266,18 +266,9 @@
     <t>Caja</t>
   </si>
   <si>
-    <t>caja</t>
-  </si>
-  <si>
     <t>local_atm</t>
   </si>
   <si>
-    <t>Inventario</t>
-  </si>
-  <si>
-    <t>inventario</t>
-  </si>
-  <si>
     <t>Caja Chica</t>
   </si>
   <si>
@@ -350,10 +341,28 @@
     <t>cierre_caja_hotel</t>
   </si>
   <si>
-    <t>Ventas</t>
-  </si>
-  <si>
-    <t>ventas-restaurante</t>
+    <t>reporte-restaurante-caja</t>
+  </si>
+  <si>
+    <t>reporte-restaurante-inventario</t>
+  </si>
+  <si>
+    <t>reporte-restaurante-venta</t>
+  </si>
+  <si>
+    <t>restaurante-caja</t>
+  </si>
+  <si>
+    <t>Reporte de caja</t>
+  </si>
+  <si>
+    <t>Reporte de inventario</t>
+  </si>
+  <si>
+    <t>Reporte de ventas</t>
+  </si>
+  <si>
+    <t>monetization_on</t>
   </si>
 </sst>
 </file>
@@ -700,10 +709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -743,16 +752,16 @@
     </row>
     <row r="2" spans="1:9" ht="21">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D2" s="4">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>15</v>
@@ -780,16 +789,16 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>15</v>
@@ -797,16 +806,16 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>15</v>
@@ -1102,10 +1111,10 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B21" t="s">
-        <v>0</v>
+        <v>108</v>
       </c>
       <c r="C21" t="s">
         <v>23</v>
@@ -1114,38 +1123,38 @@
         <v>1</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>1</v>
+        <v>112</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="4" t="s">
-        <v>79</v>
+      <c r="A22" t="s">
+        <v>78</v>
       </c>
       <c r="B22" t="s">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="D22" s="4">
         <v>1</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="F22" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="4" t="s">
-        <v>82</v>
+        <v>109</v>
       </c>
       <c r="B23" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="C23" t="s">
         <v>78</v>
@@ -1154,7 +1163,7 @@
         <v>1</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>15</v>
@@ -1162,10 +1171,10 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B24" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C24" t="s">
         <v>78</v>
@@ -1181,37 +1190,37 @@
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" t="s">
-        <v>39</v>
+      <c r="A25" s="4" t="s">
+        <v>111</v>
       </c>
       <c r="B25" t="s">
-        <v>0</v>
+        <v>107</v>
+      </c>
+      <c r="C25" t="s">
+        <v>78</v>
       </c>
       <c r="D25" s="4">
         <v>1</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>97</v>
+        <v>39</v>
       </c>
       <c r="B26" t="s">
-        <v>98</v>
-      </c>
-      <c r="C26" t="s">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="D26" s="4">
         <v>1</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>99</v>
+        <v>52</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>15</v>
@@ -1219,10 +1228,10 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>95</v>
       </c>
       <c r="C27" t="s">
         <v>39</v>
@@ -1231,7 +1240,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>15</v>
@@ -1239,10 +1248,10 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C28" t="s">
         <v>39</v>
@@ -1251,7 +1260,7 @@
         <v>1</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>15</v>
@@ -1259,10 +1268,10 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B29" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C29" t="s">
         <v>39</v>
@@ -1271,7 +1280,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>15</v>
@@ -1279,10 +1288,10 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C30" t="s">
         <v>39</v>
@@ -1291,7 +1300,7 @@
         <v>1</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>15</v>
@@ -1299,10 +1308,10 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="C31" t="s">
         <v>39</v>
@@ -1311,7 +1320,7 @@
         <v>1</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>15</v>
@@ -1319,19 +1328,19 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B32" t="s">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C32" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="D32" s="4">
         <v>1</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>15</v>
@@ -1339,10 +1348,10 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C33" t="s">
         <v>57</v>
@@ -1351,7 +1360,7 @@
         <v>1</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>15</v>
@@ -1359,10 +1368,10 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B34" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C34" t="s">
         <v>57</v>
@@ -1371,7 +1380,7 @@
         <v>1</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>15</v>
@@ -1379,10 +1388,10 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C35" t="s">
         <v>57</v>
@@ -1391,7 +1400,7 @@
         <v>1</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>15</v>
@@ -1399,10 +1408,10 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C36" t="s">
         <v>57</v>
@@ -1411,7 +1420,7 @@
         <v>1</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>15</v>
@@ -1419,10 +1428,10 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C37" t="s">
         <v>57</v>
@@ -1430,8 +1439,8 @@
       <c r="D37" s="4">
         <v>1</v>
       </c>
-      <c r="E37" t="s">
-        <v>70</v>
+      <c r="E37" s="6" t="s">
+        <v>75</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>15</v>
@@ -1439,19 +1448,19 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="B38" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="C38" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="D38" s="4">
         <v>1</v>
       </c>
-      <c r="E38" s="6" t="s">
-        <v>91</v>
+      <c r="E38" t="s">
+        <v>70</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>15</v>
@@ -1459,19 +1468,19 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="B39" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C39" t="s">
         <v>39</v>
       </c>
       <c r="D39" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>15</v>
@@ -1479,10 +1488,10 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B40" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C40" t="s">
         <v>39</v>
@@ -1491,7 +1500,7 @@
         <v>0</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>15</v>
@@ -1499,19 +1508,19 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="B41" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="C41" t="s">
         <v>39</v>
       </c>
       <c r="D41" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>15</v>
@@ -1519,18 +1528,38 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B42" t="s">
         <v>93</v>
       </c>
+      <c r="C42" t="s">
+        <v>39</v>
+      </c>
       <c r="D42" s="4">
         <v>1</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F42" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>89</v>
+      </c>
+      <c r="B43" t="s">
+        <v>90</v>
+      </c>
+      <c r="D43" s="4">
+        <v>1</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Visualizacion de cierre de caja por rol
</commit_message>
<xml_diff>
--- a/backend/database/seeders/Catalogos/RolMenu.xlsx
+++ b/backend/database/seeders/Catalogos/RolMenu.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="114">
   <si>
     <t>#</t>
   </si>
@@ -360,6 +360,12 @@
   </si>
   <si>
     <t>reporte_restaurante_venta</t>
+  </si>
+  <si>
+    <t>Apertura caja restaurante</t>
+  </si>
+  <si>
+    <t>apertura_caja_restaurante</t>
   </si>
 </sst>
 </file>
@@ -706,10 +712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1207,37 +1213,37 @@
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" t="s">
-        <v>39</v>
+      <c r="A26" s="4" t="s">
+        <v>112</v>
       </c>
       <c r="B26" t="s">
+        <v>113</v>
+      </c>
+      <c r="C26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="4">
         <v>0</v>
       </c>
-      <c r="D26" s="4">
-        <v>1</v>
-      </c>
       <c r="E26" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F26" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F26" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>93</v>
+        <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>94</v>
-      </c>
-      <c r="C27" t="s">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="D27" s="4">
         <v>1</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>95</v>
+        <v>52</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>15</v>
@@ -1245,10 +1251,10 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>94</v>
       </c>
       <c r="C28" t="s">
         <v>39</v>
@@ -1257,7 +1263,7 @@
         <v>1</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>53</v>
+        <v>95</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>15</v>
@@ -1265,10 +1271,10 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B29" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C29" t="s">
         <v>39</v>
@@ -1277,7 +1283,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>15</v>
@@ -1285,10 +1291,10 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B30" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C30" t="s">
         <v>39</v>
@@ -1297,7 +1303,7 @@
         <v>1</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>15</v>
@@ -1305,10 +1311,10 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C31" t="s">
         <v>39</v>
@@ -1317,7 +1323,7 @@
         <v>1</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>15</v>
@@ -1325,10 +1331,10 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B32" t="s">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="C32" t="s">
         <v>39</v>
@@ -1337,7 +1343,7 @@
         <v>1</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>15</v>
@@ -1345,19 +1351,19 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C33" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="D33" s="4">
         <v>1</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>15</v>
@@ -1365,10 +1371,10 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B34" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C34" t="s">
         <v>57</v>
@@ -1377,7 +1383,7 @@
         <v>1</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>15</v>
@@ -1385,10 +1391,10 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B35" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C35" t="s">
         <v>57</v>
@@ -1397,7 +1403,7 @@
         <v>1</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>15</v>
@@ -1405,10 +1411,10 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C36" t="s">
         <v>57</v>
@@ -1417,7 +1423,7 @@
         <v>1</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>15</v>
@@ -1425,10 +1431,10 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B37" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C37" t="s">
         <v>57</v>
@@ -1437,7 +1443,7 @@
         <v>1</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>15</v>
@@ -1445,10 +1451,10 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C38" t="s">
         <v>57</v>
@@ -1456,8 +1462,8 @@
       <c r="D38" s="4">
         <v>1</v>
       </c>
-      <c r="E38" t="s">
-        <v>70</v>
+      <c r="E38" s="6" t="s">
+        <v>75</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>15</v>
@@ -1465,19 +1471,19 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B39" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="C39" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="D39" s="4">
         <v>1</v>
       </c>
-      <c r="E39" s="6" t="s">
-        <v>87</v>
+      <c r="E39" t="s">
+        <v>70</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>15</v>
@@ -1485,16 +1491,16 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="B40" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C40" t="s">
         <v>39</v>
       </c>
       <c r="D40" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>87</v>
@@ -1505,10 +1511,10 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B41" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C41" t="s">
         <v>39</v>
@@ -1525,19 +1531,19 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="B42" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="C42" t="s">
         <v>39</v>
       </c>
       <c r="D42" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>15</v>
@@ -1545,18 +1551,38 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" t="s">
+        <v>92</v>
+      </c>
+      <c r="C43" t="s">
+        <v>39</v>
+      </c>
+      <c r="D43" s="4">
+        <v>1</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
         <v>88</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>89</v>
       </c>
-      <c r="D43" s="4">
-        <v>1</v>
-      </c>
-      <c r="E43" s="6" t="s">
+      <c r="D44" s="4">
+        <v>1</v>
+      </c>
+      <c r="E44" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="F44" s="1" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cierre de caja hotel
</commit_message>
<xml_diff>
--- a/backend/database/seeders/Catalogos/RolMenu.xlsx
+++ b/backend/database/seeders/Catalogos/RolMenu.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\restaurante-hotel\backend\database\seeders\Catalogos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\hotel_restuarante\backend\database\seeders\Catalogos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="112">
   <si>
     <t>#</t>
   </si>
@@ -50,12 +50,6 @@
     <t>COMBINACION (5)</t>
   </si>
   <si>
-    <t>Cátalogo General</t>
-  </si>
-  <si>
-    <t>view_module</t>
-  </si>
-  <si>
     <t>usuarios</t>
   </si>
   <si>
@@ -65,12 +59,6 @@
     <t>Usuarios</t>
   </si>
   <si>
-    <t>Ayuda</t>
-  </si>
-  <si>
-    <t>ayuda</t>
-  </si>
-  <si>
     <t>ADMIN_GERENTE</t>
   </si>
   <si>
@@ -89,12 +77,6 @@
     <t>account_circle</t>
   </si>
   <si>
-    <t>Presentaciones</t>
-  </si>
-  <si>
-    <t>presentaciones</t>
-  </si>
-  <si>
     <t>Restaurante</t>
   </si>
   <si>
@@ -372,6 +354,12 @@
   </si>
   <si>
     <t>reporte_restaurante_gastos</t>
+  </si>
+  <si>
+    <t>Cierre caja restaurante</t>
+  </si>
+  <si>
+    <t>cierre_caja_restaurante</t>
   </si>
 </sst>
 </file>
@@ -718,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -761,19 +749,19 @@
     </row>
     <row r="2" spans="1:9" ht="21">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D2" s="4">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -781,58 +769,58 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
@@ -841,181 +829,187 @@
         <v>1</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D7" s="4">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D8" s="4">
         <v>1</v>
       </c>
-      <c r="E8" t="s">
-        <v>9</v>
+      <c r="E8" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
       </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
       <c r="D9" s="4">
         <v>1</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
       </c>
-      <c r="E10" t="s">
-        <v>1</v>
+      <c r="E10" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>70</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>1</v>
+        <v>71</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D13" s="4">
         <v>1</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="D15" s="4">
         <v>1</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>77</v>
+        <v>44</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1026,373 +1020,373 @@
         <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="D16" s="4">
         <v>1</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="D17" s="4">
         <v>1</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>102</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>50</v>
+        <v>101</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D19" s="4">
         <v>1</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" t="s">
-        <v>32</v>
+      <c r="A20" s="4" t="s">
+        <v>98</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>103</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>15</v>
+        <v>71</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" t="s">
-        <v>79</v>
+      <c r="A21" s="4" t="s">
+        <v>99</v>
       </c>
       <c r="B21" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="D21" s="4">
         <v>1</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>15</v>
+        <v>71</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" t="s">
-        <v>78</v>
+      <c r="A22" s="4" t="s">
+        <v>100</v>
       </c>
       <c r="B22" t="s">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="C22" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="D22" s="4">
         <v>1</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>15</v>
+        <v>71</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="4" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B23" t="s">
         <v>109</v>
       </c>
       <c r="C23" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D23" s="4">
         <v>1</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B24" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C24" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
       <c r="D24" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="4" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B25" t="s">
         <v>111</v>
       </c>
       <c r="C25" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
       <c r="D25" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="4" t="s">
-        <v>114</v>
+      <c r="A26" t="s">
+        <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>115</v>
-      </c>
-      <c r="C26" t="s">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="D26" s="4">
         <v>1</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>15</v>
+        <v>46</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="4" t="s">
-        <v>112</v>
+      <c r="A27" t="s">
+        <v>87</v>
       </c>
       <c r="B27" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
       <c r="C27" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="D27" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>15</v>
+        <v>89</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>0</v>
+        <v>35</v>
+      </c>
+      <c r="C28" t="s">
+        <v>33</v>
       </c>
       <c r="D28" s="4">
         <v>1</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>93</v>
+        <v>36</v>
       </c>
       <c r="B29" t="s">
-        <v>94</v>
+        <v>37</v>
       </c>
       <c r="C29" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D29" s="4">
         <v>1</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>95</v>
+        <v>48</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" t="s">
         <v>40</v>
       </c>
-      <c r="B30" t="s">
-        <v>41</v>
-      </c>
       <c r="C30" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D30" s="4">
         <v>1</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C31" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D31" s="4">
         <v>1</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B32" t="s">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="C32" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D32" s="4">
         <v>1</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B33" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C33" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D33" s="4">
         <v>1</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" t="s">
         <v>57</v>
       </c>
-      <c r="B34" t="s">
-        <v>0</v>
-      </c>
       <c r="C34" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D34" s="4">
         <v>1</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1400,216 +1394,176 @@
         <v>59</v>
       </c>
       <c r="B35" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35" s="4">
+        <v>1</v>
+      </c>
+      <c r="E35" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C35" t="s">
-        <v>57</v>
-      </c>
-      <c r="D35" s="4">
-        <v>1</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>64</v>
-      </c>
       <c r="F35" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B36" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C36" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D36" s="4">
         <v>1</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B37" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C37" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D37" s="4">
         <v>1</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B38" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C38" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D38" s="4">
         <v>1</v>
       </c>
-      <c r="E38" s="6" t="s">
-        <v>51</v>
+      <c r="E38" t="s">
+        <v>64</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B39" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="C39" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="D39" s="4">
         <v>1</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="B40" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="C40" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="D40" s="4">
-        <v>1</v>
-      </c>
-      <c r="E40" t="s">
-        <v>70</v>
+        <v>0</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="B41" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C41" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D41" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>99</v>
+        <v>72</v>
       </c>
       <c r="B42" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="C42" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D42" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="B43" t="s">
-        <v>103</v>
-      </c>
-      <c r="C43" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="D43" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" t="s">
-        <v>78</v>
-      </c>
-      <c r="B44" t="s">
-        <v>92</v>
-      </c>
-      <c r="C44" t="s">
-        <v>39</v>
-      </c>
-      <c r="D44" s="4">
-        <v>1</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B45" t="s">
-        <v>89</v>
-      </c>
-      <c r="D45" s="4">
-        <v>1</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>